<commit_message>
Submitted Current work and updated documents
</commit_message>
<xml_diff>
--- a/Project Documents/Sprint_Planning_Document_CS492.xlsx
+++ b/Project Documents/Sprint_Planning_Document_CS492.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gallo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gallo\Documents\GitHub\CS492\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D87B8D-FED7-41B1-A9E3-B6BFE5955847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F8F94C-C628-49C2-BFB4-639FA5F93DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="hidden" r:id="rId1"/>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="280">
   <si>
     <t>Project Name</t>
   </si>
@@ -912,6 +912,12 @@
   </si>
   <si>
     <t>User Story</t>
+  </si>
+  <si>
+    <t>T-779</t>
+  </si>
+  <si>
+    <t>We need to create a Mongo DB Schema that contains all of the Admin Page including the password, change logs, and current sales</t>
   </si>
 </sst>
 </file>
@@ -2378,7 +2384,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$G$50:$T$50</c:f>
+              <c:f>'Sprint 1'!$G$51:$T$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2467,7 +2473,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$G$51:$T$51</c:f>
+              <c:f>'Sprint 1'!$G$52:$T$52</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="14"/>
@@ -3468,13 +3474,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>92784</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>154305</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4026,8 +4032,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -4038,8 +4044,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -5667,26 +5673,26 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{F20B8E5E-54BC-4256-9FEF-E7941184C71C}"/>
+      <autoFilter ref="B1:F1" xr:uid="{9BD8C0CA-70A1-4A29-A35C-62E3CF1ECC10}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{96E4222B-7FF1-417B-82DD-C671983F980E}"/>
+      <autoFilter ref="B1:F1" xr:uid="{7D4BB6F7-85A5-42EB-AD68-3EC329A394FC}"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{6D7ACFEF-E691-4516-A0CC-0B70E7D8B8F1}"/>
+      <autoFilter ref="B1:F1" xr:uid="{40D91298-7A78-4407-9CCA-94FA15BA1F69}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -5708,12 +5714,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AAAAEB-B5F0-468C-BFDD-E9B5D3EFF0AD}">
-  <dimension ref="B1:T73"/>
+  <dimension ref="B1:T74"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6191,7 +6197,9 @@
       <c r="K18" s="52"/>
       <c r="L18" s="52"/>
       <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
+      <c r="N18" s="52">
+        <v>2</v>
+      </c>
       <c r="O18" s="52"/>
       <c r="P18" s="52"/>
       <c r="Q18" s="52"/>
@@ -6292,7 +6300,9 @@
       <c r="O21" s="38"/>
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
+      <c r="R21" s="38">
+        <v>2</v>
+      </c>
       <c r="S21" s="38"/>
       <c r="T21" s="38"/>
     </row>
@@ -6413,7 +6423,9 @@
       <c r="J25" s="38"/>
       <c r="K25" s="38"/>
       <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
+      <c r="M25" s="38">
+        <v>2</v>
+      </c>
       <c r="N25" s="38"/>
       <c r="O25" s="38"/>
       <c r="P25" s="38"/>
@@ -6432,7 +6444,9 @@
       <c r="D26" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="51"/>
+      <c r="E26" s="51" t="s">
+        <v>18</v>
+      </c>
       <c r="F26" s="52">
         <v>3</v>
       </c>
@@ -6445,7 +6459,9 @@
       <c r="M26" s="52"/>
       <c r="N26" s="52"/>
       <c r="O26" s="52"/>
-      <c r="P26" s="52"/>
+      <c r="P26" s="52">
+        <v>4</v>
+      </c>
       <c r="Q26" s="52"/>
       <c r="R26" s="52"/>
       <c r="S26" s="52"/>
@@ -6635,7 +6651,9 @@
       <c r="D33" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="E33" s="38" t="s">
+        <v>50</v>
+      </c>
       <c r="F33" s="38">
         <v>3</v>
       </c>
@@ -6649,7 +6667,9 @@
       <c r="N33" s="38"/>
       <c r="O33" s="38"/>
       <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
+      <c r="Q33" s="38">
+        <v>2.5</v>
+      </c>
       <c r="R33" s="38"/>
       <c r="S33" s="38"/>
       <c r="T33" s="38"/>
@@ -6722,7 +6742,9 @@
       <c r="D36" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="51"/>
+      <c r="E36" s="51" t="s">
+        <v>17</v>
+      </c>
       <c r="F36" s="52">
         <v>3</v>
       </c>
@@ -6734,7 +6756,9 @@
       <c r="L36" s="52"/>
       <c r="M36" s="52"/>
       <c r="N36" s="52"/>
-      <c r="O36" s="52"/>
+      <c r="O36" s="52">
+        <v>1.5</v>
+      </c>
       <c r="P36" s="52"/>
       <c r="Q36" s="52"/>
       <c r="R36" s="52"/>
@@ -6751,7 +6775,9 @@
       <c r="D37" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="51" t="s">
+        <v>273</v>
+      </c>
       <c r="F37" s="38">
         <v>3</v>
       </c>
@@ -6766,7 +6792,9 @@
       <c r="O37" s="38"/>
       <c r="P37" s="38"/>
       <c r="Q37" s="38"/>
-      <c r="R37" s="38"/>
+      <c r="R37" s="38">
+        <v>5</v>
+      </c>
       <c r="S37" s="38"/>
       <c r="T37" s="38"/>
     </row>
@@ -7016,7 +7044,9 @@
       <c r="D46" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="51"/>
+      <c r="E46" s="51" t="s">
+        <v>50</v>
+      </c>
       <c r="F46" s="52">
         <v>3</v>
       </c>
@@ -7029,7 +7059,9 @@
       <c r="M46" s="52"/>
       <c r="N46" s="52"/>
       <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
+      <c r="P46" s="52">
+        <v>2</v>
+      </c>
       <c r="Q46" s="52"/>
       <c r="R46" s="52"/>
       <c r="S46" s="52"/>
@@ -7045,7 +7077,9 @@
       <c r="D47" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="38"/>
+      <c r="E47" s="38" t="s">
+        <v>273</v>
+      </c>
       <c r="F47" s="38">
         <v>3</v>
       </c>
@@ -7057,7 +7091,9 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
-      <c r="O47" s="38"/>
+      <c r="O47" s="38">
+        <v>4</v>
+      </c>
       <c r="P47" s="38"/>
       <c r="Q47" s="38"/>
       <c r="R47" s="38"/>
@@ -7097,126 +7133,150 @@
       <c r="S48" s="52"/>
       <c r="T48" s="52"/>
     </row>
-    <row r="49" spans="4:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-    </row>
-    <row r="50" spans="4:20" s="45" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="46" t="s">
+    <row r="49" spans="2:20" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="52" t="s">
+        <v>278</v>
+      </c>
+      <c r="C49" s="52">
+        <v>77</v>
+      </c>
+      <c r="D49" s="53" t="s">
+        <v>279</v>
+      </c>
+      <c r="E49" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" s="52">
+        <v>2</v>
+      </c>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="52"/>
+      <c r="P49" s="52"/>
+      <c r="Q49" s="52">
+        <v>2</v>
+      </c>
+      <c r="R49" s="52"/>
+      <c r="S49" s="52"/>
+      <c r="T49" s="52"/>
+    </row>
+    <row r="50" spans="2:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+    </row>
+    <row r="51" spans="2:20" s="45" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="E50" s="47"/>
-      <c r="F50" s="77">
+      <c r="E51" s="47"/>
+      <c r="F51" s="77">
         <f>8*2*C7</f>
         <v>80</v>
       </c>
-      <c r="G50" s="48" t="e">
+      <c r="G51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H50" s="48" t="e">
+      <c r="H51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I50" s="48" t="e">
+      <c r="I51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J50" s="48" t="e">
+      <c r="J51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K50" s="48" t="e">
+      <c r="K51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L50" s="48" t="e">
+      <c r="L51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M50" s="48" t="e">
+      <c r="M51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N50" s="48" t="e">
+      <c r="N51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="O50" s="48" t="e">
+      <c r="O51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P50" s="48" t="e">
+      <c r="P51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="Q50" s="48" t="e">
+      <c r="Q51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R50" s="48" t="e">
+      <c r="R51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="S50" s="48" t="e">
+      <c r="S51" s="48" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T50" s="48" t="e">
+      <c r="T51" s="48" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="4:20" s="45" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="46" t="s">
+    <row r="52" spans="2:20" s="45" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="49"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="50">
+      <c r="E52" s="49"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="50">
         <v>44.571428571428569</v>
       </c>
-      <c r="H51" s="50">
+      <c r="H52" s="50">
         <v>41.142857142857139</v>
       </c>
-      <c r="I51" s="50">
+      <c r="I52" s="50">
         <v>37.714285714285708</v>
       </c>
-      <c r="J51" s="50">
+      <c r="J52" s="50">
         <v>34.285714285714278</v>
       </c>
-      <c r="K51" s="50">
+      <c r="K52" s="50">
         <v>30.857142857142851</v>
       </c>
-      <c r="L51" s="50">
+      <c r="L52" s="50">
         <v>27.428571428571423</v>
       </c>
-      <c r="M51" s="50">
+      <c r="M52" s="50">
         <v>23.999999999999996</v>
       </c>
-      <c r="N51" s="50">
+      <c r="N52" s="50">
         <v>20.571428571428569</v>
       </c>
-      <c r="O51" s="50">
+      <c r="O52" s="50">
         <v>17.142857142857142</v>
       </c>
-      <c r="P51" s="50">
+      <c r="P52" s="50">
         <v>13.714285714285714</v>
       </c>
-      <c r="Q51" s="50">
+      <c r="Q52" s="50">
         <v>10.285714285714285</v>
       </c>
-      <c r="R51" s="50">
+      <c r="R52" s="50">
         <v>6.8571428571428559</v>
       </c>
-      <c r="S51" s="50">
+      <c r="S52" s="50">
         <v>3.4285714285714275</v>
       </c>
-      <c r="T51" s="50">
+      <c r="T52" s="50">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-    </row>
-    <row r="53" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -7225,7 +7285,7 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
     </row>
-    <row r="54" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -7234,19 +7294,16 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
     </row>
-    <row r="55" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-    </row>
-    <row r="56" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -7258,7 +7315,7 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -7270,7 +7327,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -7282,7 +7339,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -7294,7 +7351,7 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -7306,7 +7363,7 @@
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
     </row>
-    <row r="61" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -7318,7 +7375,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -7330,7 +7387,7 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -7342,7 +7399,7 @@
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -7379,13 +7436,16 @@
       <c r="M66" s="3"/>
     </row>
     <row r="67" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
-      <c r="S67" s="2"/>
-      <c r="T67" s="2"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
     </row>
     <row r="68" spans="4:20" x14ac:dyDescent="0.2">
       <c r="N68" s="2"/>
@@ -7441,13 +7501,22 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
     </row>
+    <row r="74" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="2"/>
+      <c r="T74" s="2"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" autoFilter="0"/>
   <autoFilter ref="B12:F12" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="8">
     <mergeCell ref="G9:M9"/>
     <mergeCell ref="N9:T9"/>
-    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F51:F52"/>
     <mergeCell ref="B2:T2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
@@ -7455,12 +7524,12 @@
     <mergeCell ref="C7:D7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="G50:T50">
+  <conditionalFormatting sqref="G51:T51">
     <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="lessThan">
-      <formula>G51</formula>
+      <formula>G52</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
-      <formula>G51</formula>
+      <formula>G52</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8903,15 +8972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CD5BF1D25B04C4DAFCC598A42891EA8" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45b73b173887e5427e1a7d1313c48df7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bbb67f6-bffc-474b-aafb-fa77ef9cf4e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d8638d06aff927da092ea6a13d6d28c" ns2:_="">
     <xsd:import namespace="2bbb67f6-bffc-474b-aafb-fa77ef9cf4e0"/>
@@ -9043,15 +9103,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE0C23A-5102-4081-835D-8A52FB2528A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554BC761-B369-43F7-8379-D7BE3B6A4E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9067,4 +9128,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE0C23A-5102-4081-835D-8A52FB2528A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>